<commit_message>
atualização planilha de requesitos
</commit_message>
<xml_diff>
--- a/Gestão/Planilha de horários reuniões.xlsx
+++ b/Gestão/Planilha de horários reuniões.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakar\Desktop\BandTec\Primeiro semestre\TurtleLife\Gestão\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4eeb03d78f3bc2b8/Área de Trabalho/Sprint 2/Sprint-2-turtlelife/Gestão/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_1CB6D3C1848F00118B2693D8064C393C1D729CC6" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB8232B1-8D15-43F5-A99D-78B5C547DC29}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Tabela de horários de reuniões</t>
   </si>
@@ -35,16 +36,19 @@
     <t>Dia</t>
   </si>
   <si>
-    <t>9h00</t>
+    <t>À definir necessidade</t>
   </si>
   <si>
-    <t>À definir necessidade</t>
+    <t>18h00</t>
+  </si>
+  <si>
+    <t>Concluida</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,7 +92,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -111,29 +115,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -415,11 +450,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,88 +462,89 @@
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="D2" s="3"/>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5">
+        <v>44109</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2">
+        <v>44115</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7">
-        <v>44082</v>
-      </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3">
-        <v>44085</v>
-      </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3">
-        <v>44088</v>
-      </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3">
-        <v>44091</v>
-      </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3">
-        <v>44093</v>
-      </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3">
-        <v>44094</v>
-      </c>
-      <c r="D8" s="4"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="A2:B2"/>
@@ -518,12 +554,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
atualização de planilha de horários/reuniões
</commit_message>
<xml_diff>
--- a/Gestão/Planilha de horários reuniões.xlsx
+++ b/Gestão/Planilha de horários reuniões.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4eeb03d78f3bc2b8/Área de Trabalho/Sprint 2/Sprint-2-turtlelife/Gestão/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_1CB6D3C1848F00118B2693D8064C393C1D729CC6" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB8232B1-8D15-43F5-A99D-78B5C547DC29}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="11_1CB6D3C1848F00118B2693D8064C393C1D729CC6" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{729630EC-1105-4C96-AA92-4B56056EF0DB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="24">
   <si>
     <t>Tabela de horários de reuniões</t>
   </si>
@@ -43,13 +43,67 @@
   </si>
   <si>
     <t>Concluida</t>
+  </si>
+  <si>
+    <t>15h15</t>
+  </si>
+  <si>
+    <t>Tabela de definição de cargos semanais</t>
+  </si>
+  <si>
+    <t>Scrum master</t>
+  </si>
+  <si>
+    <t>Caique</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>Lais</t>
+  </si>
+  <si>
+    <t>Develvolvedor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analista </t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Rafael</t>
+  </si>
+  <si>
+    <t>luis</t>
+  </si>
+  <si>
+    <t>Leonardo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Semana do dia 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  semana do dia 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  semana do dia 19</t>
+  </si>
+  <si>
+    <t>A definir</t>
+  </si>
+  <si>
+    <t>Presente</t>
+  </si>
+  <si>
+    <t>Nome</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +115,12 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -141,18 +201,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -162,15 +261,13 @@
     <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,98 +548,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="0.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="I1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="F2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="D2" s="13"/>
+      <c r="I2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5">
+      <c r="B3" s="14"/>
+      <c r="C3" s="15">
         <v>44109</v>
       </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="14"/>
+      <c r="I3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2">
+      <c r="B4" s="14"/>
+      <c r="C4" s="15">
         <v>44115</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="D4" s="14"/>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="15">
+        <v>44117</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="I5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="I6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="I7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="1"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="I8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3">
+        <v>44109</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44115</v>
+      </c>
+      <c r="D9" s="3">
+        <v>44117</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="19">
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I9:L9"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="A8:B8"/>
@@ -554,7 +874,10 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Inclui a tabela riscos
</commit_message>
<xml_diff>
--- a/Gestão/Planilha de horários reuniões.xlsx
+++ b/Gestão/Planilha de horários reuniões.xlsx
@@ -237,37 +237,37 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,7 +551,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,50 +564,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="I1" s="8" t="s">
+      <c r="F1" s="10"/>
+      <c r="I1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="I2" s="8" t="s">
+      <c r="D2" s="16"/>
+      <c r="I2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15">
+      <c r="B3" s="10"/>
+      <c r="C3" s="9">
         <v>44109</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="10"/>
       <c r="I3" s="7" t="s">
         <v>8</v>
       </c>
@@ -618,14 +618,14 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15">
+      <c r="B4" s="10"/>
+      <c r="C4" s="9">
         <v>44115</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="10"/>
       <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
@@ -636,14 +636,14 @@
       <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="15">
+      <c r="B5" s="18"/>
+      <c r="C5" s="9">
         <v>44117</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="10"/>
       <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
@@ -654,12 +654,12 @@
       <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
       <c r="I6" s="2" t="s">
         <v>12</v>
       </c>
@@ -670,12 +670,12 @@
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
       <c r="I7" s="2" t="s">
         <v>12</v>
       </c>
@@ -686,12 +686,12 @@
       <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
       <c r="I8" s="2" t="s">
         <v>13</v>
       </c>
@@ -702,7 +702,7 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="3">
@@ -714,14 +714,14 @@
       <c r="D9" s="3">
         <v>44117</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -857,16 +857,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>

</xml_diff>

<commit_message>
inclui a pagina de configurações e suporte
</commit_message>
<xml_diff>
--- a/Gestão/Planilha de horários reuniões.xlsx
+++ b/Gestão/Planilha de horários reuniões.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4eeb03d78f3bc2b8/Área de Trabalho/Sprint 2/Sprint-2-turtlelife/Gestão/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="11_1CB6D3C1848F00118B2693D8064C393C1D729CC6" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{729630EC-1105-4C96-AA92-4B56056EF0DB}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="11_1CB6D3C1848F00118B2693D8064C393C1D729CC6" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2F869DFC-2546-4CE2-B8DE-567BBFB3B63B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
   <si>
     <t>Tabela de horários de reuniões</t>
   </si>
@@ -90,20 +90,23 @@
     <t xml:space="preserve">  semana do dia 19</t>
   </si>
   <si>
-    <t>A definir</t>
-  </si>
-  <si>
     <t>Presente</t>
   </si>
   <si>
     <t>Nome</t>
+  </si>
+  <si>
+    <t>josé</t>
+  </si>
+  <si>
+    <t>19h31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +124,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -238,27 +249,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -266,6 +277,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -551,35 +565,36 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="8" max="8" width="0.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="0.28515625" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="9" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="I1" s="15" t="s">
+      <c r="F1" s="15"/>
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -590,24 +605,24 @@
         <v>2</v>
       </c>
       <c r="D2" s="16"/>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="9">
+      <c r="B3" s="15"/>
+      <c r="C3" s="14">
         <v>44109</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="15"/>
       <c r="I3" s="7" t="s">
         <v>8</v>
       </c>
@@ -618,14 +633,14 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="9">
+      <c r="B4" s="15"/>
+      <c r="C4" s="14">
         <v>44115</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="15"/>
       <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
@@ -640,10 +655,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="18"/>
-      <c r="C5" s="9">
+      <c r="C5" s="14">
         <v>44117</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="15"/>
       <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
@@ -654,12 +669,14 @@
       <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
+      <c r="A6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="14">
+        <v>44119</v>
+      </c>
+      <c r="D6" s="15"/>
       <c r="I6" s="2" t="s">
         <v>12</v>
       </c>
@@ -670,12 +687,14 @@
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
+      <c r="A7" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="14">
+        <v>44124</v>
+      </c>
+      <c r="D7" s="15"/>
       <c r="I7" s="2" t="s">
         <v>12</v>
       </c>
@@ -686,12 +705,12 @@
       <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
       <c r="I8" s="2" t="s">
         <v>13</v>
       </c>
@@ -703,7 +722,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3">
         <v>44109</v>
@@ -714,33 +733,33 @@
       <c r="D9" s="3">
         <v>44117</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -750,19 +769,19 @@
         <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -772,19 +791,19 @@
         <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -794,19 +813,19 @@
         <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -816,19 +835,19 @@
         <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>21</v>
+      <c r="J14" s="19" t="s">
+        <v>11</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
@@ -838,30 +857,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
@@ -876,8 +890,14 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>